<commit_message>
Added pkl and excel of code in master2
</commit_message>
<xml_diff>
--- a/Assign_2/output/routes.xlsx
+++ b/Assign_2/output/routes.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Day 1 - 0 h 42</t>
+          <t>Day 1 - 23 h 42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -478,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Day 2 - -20 h 54</t>
+          <t>Day 2 - 3 h 54</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -491,7 +491,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Day 2 - -20 h 54</t>
+          <t>Day 2 - 3 h 54</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day 2 - -15 h 6</t>
+          <t>Day 2 - 8 h 6</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -514,7 +514,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Day 2 - -12 h 54</t>
+          <t>Day 2 - 11 h 54</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -524,7 +524,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Day 2 - -8 h 24</t>
+          <t>Day 2 - 15 h 24</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -537,7 +537,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Day 2 - -4 h 0</t>
+          <t>Day 2 - 20 h 0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -547,7 +547,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Day 2 - 0 h 30</t>
+          <t>Day 2 - 23 h 30</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -560,7 +560,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Day 3 - -23 h 24</t>
+          <t>Day 3 - 0 h 24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -570,7 +570,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 54</t>
+          <t>Day 3 - 3 h 54</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -583,7 +583,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 54</t>
+          <t>Day 3 - 3 h 54</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Day 3 - -16 h 24</t>
+          <t>Day 3 - 7 h 24</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -606,7 +606,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Day 4 - -20 h 54</t>
+          <t>Day 4 - 3 h 54</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Day 4 - -15 h 6</t>
+          <t>Day 4 - 8 h 6</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -629,7 +629,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Day 5 - -20 h 0</t>
+          <t>Day 5 - 4 h 0</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Day 5 - -15 h 12</t>
+          <t>Day 5 - 8 h 12</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -698,7 +698,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Day 2 - -21 h 54</t>
+          <t>Day 2 - 2 h 54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -708,7 +708,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Day 2 - -16 h 54</t>
+          <t>Day 2 - 7 h 54</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -721,7 +721,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Day 2 - -16 h 54</t>
+          <t>Day 2 - 7 h 54</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -731,7 +731,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day 2 - -11 h 54</t>
+          <t>Day 2 - 12 h 54</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -744,7 +744,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Day 2 - 0 h 54</t>
+          <t>Day 2 - 23 h 54</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Day 3 - -19 h 54</t>
+          <t>Day 3 - 4 h 54</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -767,7 +767,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Day 4 - -24 h 0</t>
+          <t>Day 4 - 0 h 0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -777,7 +777,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Day 4 - -19 h 0</t>
+          <t>Day 4 - 5 h 0</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -790,7 +790,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Day 4 - -16 h 54</t>
+          <t>Day 4 - 7 h 54</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -800,7 +800,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Day 4 - -12 h 18</t>
+          <t>Day 4 - 11 h 18</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -813,7 +813,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Day 4 - -4 h 0</t>
+          <t>Day 4 - 20 h 0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Day 4 - 0 h 24</t>
+          <t>Day 4 - 23 h 24</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -836,7 +836,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Day 4 - 0 h 54</t>
+          <t>Day 4 - 23 h 54</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Day 5 - -19 h 18</t>
+          <t>Day 5 - 4 h 18</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -859,7 +859,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Day 5 - -19 h 18</t>
+          <t>Day 5 - 4 h 18</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -869,7 +869,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Day 5 - -15 h 42</t>
+          <t>Day 5 - 8 h 42</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -928,7 +928,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Day 2 - -20 h 54</t>
+          <t>Day 2 - 3 h 54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -938,7 +938,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Day 2 - -16 h 18</t>
+          <t>Day 2 - 7 h 18</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -951,7 +951,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Day 2 - -4 h 0</t>
+          <t>Day 2 - 20 h 0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day 2 - 0 h 24</t>
+          <t>Day 2 - 23 h 24</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -974,7 +974,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Day 2 - 0 h 30</t>
+          <t>Day 2 - 23 h 30</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -984,7 +984,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 54</t>
+          <t>Day 3 - 3 h 54</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -997,7 +997,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 54</t>
+          <t>Day 3 - 3 h 54</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Day 3 - -15 h 18</t>
+          <t>Day 3 - 8 h 18</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1020,7 +1020,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Day 3 - -2 h 42</t>
+          <t>Day 3 - 21 h 42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Day 4 - -22 h 6</t>
+          <t>Day 4 - 1 h 6</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -1043,7 +1043,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Day 4 - -22 h 6</t>
+          <t>Day 4 - 1 h 6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Day 4 - -19 h 30</t>
+          <t>Day 4 - 4 h 30</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1066,7 +1066,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Day 4 - -19 h 30</t>
+          <t>Day 4 - 4 h 30</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Day 4 - -16 h 54</t>
+          <t>Day 4 - 7 h 54</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -1089,7 +1089,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Day 4 - -16 h 54</t>
+          <t>Day 4 - 7 h 54</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Day 4 - -12 h 18</t>
+          <t>Day 4 - 11 h 18</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -1112,7 +1112,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Day 4 - -3 h 48</t>
+          <t>Day 4 - 20 h 48</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1122,7 +1122,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Day 4 - 0 h 54</t>
+          <t>Day 4 - 23 h 54</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1135,7 +1135,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Day 4 - 0 h 54</t>
+          <t>Day 4 - 23 h 54</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1145,7 +1145,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Day 5 - -21 h 0</t>
+          <t>Day 5 - 3 h 0</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1158,7 +1158,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Day 5 - -19 h 12</t>
+          <t>Day 5 - 4 h 12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Day 5 - -16 h 54</t>
+          <t>Day 5 - 7 h 54</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1181,7 +1181,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Day 5 - -16 h 54</t>
+          <t>Day 5 - 7 h 54</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Day 5 - -12 h 36</t>
+          <t>Day 5 - 11 h 36</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1250,7 +1250,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Day 2 - 0 h 54</t>
+          <t>Day 2 - 23 h 54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 0</t>
+          <t>Day 3 - 4 h 0</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1273,7 +1273,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Day 3 - -4 h 0</t>
+          <t>Day 3 - 20 h 0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day 4 - -23 h 6</t>
+          <t>Day 4 - 0 h 6</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1296,7 +1296,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Day 4 - -20 h 54</t>
+          <t>Day 4 - 3 h 54</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1306,7 +1306,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Day 4 - -15 h 12</t>
+          <t>Day 4 - 8 h 12</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1319,7 +1319,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Day 5 - -20 h 0</t>
+          <t>Day 5 - 4 h 0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Day 5 - -15 h 18</t>
+          <t>Day 5 - 8 h 18</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1388,7 +1388,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Day 3 - -20 h 54</t>
+          <t>Day 3 - 3 h 54</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Day 3 - -16 h 30</t>
+          <t>Day 3 - 7 h 30</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1411,7 +1411,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Day 4 - -20 h 0</t>
+          <t>Day 4 - 4 h 0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day 4 - -16 h 36</t>
+          <t>Day 4 - 7 h 36</t>
         </is>
       </c>
       <c r="D3" t="n">

</xml_diff>